<commit_message>
Rework of cycle tables
</commit_message>
<xml_diff>
--- a/ixp_app/data/raw/resin.xlsx
+++ b/ixp_app/data/raw/resin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjordan\ProgramingProjects\IX_Performance_Platform\ixp_app\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F1E63B-54FD-43D5-9940-685CEFC8CB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D2DF3-920C-40E2-B496-6A4A84773844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7DA27F4-7EAF-4133-8F3E-632D09353173}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7DA27F4-7EAF-4133-8F3E-632D09353173}"/>
   </bookViews>
   <sheets>
     <sheet name="ResinReplacments" sheetId="3" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="139">
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>41IXA</t>
   </si>
   <si>
@@ -453,6 +450,9 @@
   </si>
   <si>
     <t>Z Anion</t>
+  </si>
+  <si>
+    <t>TS</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,7 +818,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,814 +831,814 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C36" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="C45" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="C46" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="C48" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="C51" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="C52" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="C53" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="C54" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="C56" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="C57" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="C58" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>